<commit_message>
Add example 17 and 18
</commit_message>
<xml_diff>
--- a/ampl-data-input-excel/17-PM.Angel/17-PM.Angel.xlsx
+++ b/ampl-data-input-excel/17-PM.Angel/17-PM.Angel.xlsx
@@ -541,7 +541,7 @@
     <numFmt numFmtId="168" formatCode="0.00"/>
     <numFmt numFmtId="169" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -588,11 +588,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -686,7 +681,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -799,10 +794,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -835,7 +826,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1028,7 +1019,7 @@
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H71" activeCellId="0" sqref="H71"/>
     </sheetView>
   </sheetViews>
@@ -1118,14 +1109,14 @@
   </sheetPr>
   <dimension ref="A1:F181"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="13.71"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="6" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="2" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="1" width="11.57"/>
@@ -1135,13 +1126,13 @@
       <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="4" t="b">
@@ -1157,7 +1148,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="1" t="n">
@@ -1179,7 +1170,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="29" t="s">
         <v>37</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -1201,7 +1192,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="31" t="s">
         <v>38</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -1223,7 +1214,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="31" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -1245,7 +1236,7 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="31" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -1267,7 +1258,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="31" t="s">
         <v>41</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -1289,7 +1280,7 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="31" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -1311,7 +1302,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="31" t="s">
         <v>43</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -1333,7 +1324,7 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="31" t="s">
         <v>44</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -1355,7 +1346,7 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="31" t="s">
         <v>45</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -1377,7 +1368,7 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="31" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -1399,7 +1390,7 @@
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="31" t="s">
         <v>47</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -1418,861 +1409,861 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="30"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="30"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="30"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20"/>
-      <c r="B17" s="30"/>
+      <c r="B17" s="29"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="20"/>
-      <c r="B18" s="30"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="20"/>
-      <c r="B19" s="30"/>
+      <c r="B19" s="29"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="20"/>
-      <c r="B20" s="30"/>
+      <c r="B20" s="29"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="20"/>
-      <c r="B21" s="30"/>
+      <c r="B21" s="29"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="20"/>
-      <c r="B22" s="30"/>
+      <c r="B22" s="29"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="20"/>
-      <c r="B23" s="30"/>
+      <c r="B23" s="29"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="20"/>
-      <c r="B24" s="30"/>
+      <c r="B24" s="29"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="20"/>
-      <c r="B25" s="30"/>
+      <c r="B25" s="29"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="20"/>
-      <c r="B26" s="30"/>
+      <c r="B26" s="29"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="20"/>
-      <c r="B27" s="30"/>
+      <c r="B27" s="29"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="20"/>
-      <c r="B28" s="30"/>
+      <c r="B28" s="29"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="20"/>
-      <c r="B29" s="30"/>
+      <c r="B29" s="29"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="20"/>
-      <c r="B30" s="30"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="20"/>
-      <c r="B31" s="30"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="20"/>
-      <c r="B32" s="30"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="20"/>
-      <c r="B33" s="30"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="20"/>
-      <c r="B34" s="30"/>
+      <c r="B34" s="29"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="20"/>
-      <c r="B35" s="30"/>
+      <c r="B35" s="29"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="32"/>
+      <c r="B36" s="31"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="32"/>
+      <c r="B37" s="31"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="30"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="30"/>
+      <c r="B39" s="29"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="32"/>
+      <c r="B40" s="31"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="32"/>
+      <c r="B41" s="31"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="32"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="32"/>
+      <c r="B43" s="31"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="32"/>
+      <c r="B44" s="31"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="32"/>
+      <c r="B45" s="31"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="32"/>
+      <c r="B46" s="31"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="32"/>
+      <c r="B47" s="31"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="32"/>
+      <c r="B48" s="31"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="32"/>
+      <c r="B49" s="31"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="30"/>
+      <c r="B50" s="29"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="30"/>
+      <c r="B51" s="29"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="32"/>
+      <c r="B52" s="31"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="32"/>
+      <c r="B53" s="31"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="32"/>
+      <c r="B54" s="31"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="32"/>
+      <c r="B55" s="31"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="32"/>
+      <c r="B56" s="31"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="32"/>
+      <c r="B57" s="31"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="32"/>
+      <c r="B58" s="31"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="32"/>
+      <c r="B59" s="31"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="32"/>
+      <c r="B60" s="31"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="32"/>
+      <c r="B61" s="31"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="30"/>
+      <c r="B62" s="29"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="30"/>
+      <c r="B63" s="29"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="32"/>
+      <c r="B64" s="31"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="32"/>
+      <c r="B65" s="31"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="32"/>
+      <c r="B66" s="31"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="32"/>
+      <c r="B67" s="31"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="32"/>
+      <c r="B68" s="31"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="32"/>
+      <c r="B69" s="31"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="32"/>
+      <c r="B70" s="31"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="32"/>
+      <c r="B71" s="31"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="32"/>
+      <c r="B72" s="31"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="32"/>
+      <c r="B73" s="31"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="30"/>
+      <c r="B74" s="29"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="30"/>
+      <c r="B75" s="29"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="32"/>
+      <c r="B76" s="31"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="32"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="32"/>
+      <c r="B78" s="31"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="32"/>
+      <c r="B79" s="31"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="32"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="32"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="32"/>
+      <c r="B82" s="31"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="32"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="32"/>
+      <c r="B84" s="31"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="32"/>
+      <c r="B85" s="31"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="30"/>
+      <c r="B86" s="29"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="30"/>
+      <c r="B87" s="29"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="32"/>
+      <c r="B88" s="31"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="32"/>
+      <c r="B89" s="31"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="32"/>
+      <c r="B90" s="31"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="32"/>
+      <c r="B91" s="31"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="32"/>
+      <c r="B92" s="31"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="32"/>
+      <c r="B93" s="31"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="32"/>
+      <c r="B94" s="31"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="32"/>
+      <c r="B95" s="31"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="32"/>
+      <c r="B96" s="31"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="32"/>
+      <c r="B97" s="31"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="30"/>
+      <c r="B98" s="29"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="30"/>
+      <c r="B99" s="29"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="32"/>
+      <c r="B100" s="31"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="32"/>
+      <c r="B101" s="31"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="32"/>
+      <c r="B102" s="31"/>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="32"/>
+      <c r="B103" s="31"/>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="32"/>
+      <c r="B104" s="31"/>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="32"/>
+      <c r="B105" s="31"/>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="32"/>
+      <c r="B106" s="31"/>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="32"/>
+      <c r="B107" s="31"/>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="32"/>
+      <c r="B108" s="31"/>
       <c r="C108" s="1"/>
       <c r="D108" s="1"/>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="32"/>
+      <c r="B109" s="31"/>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="30"/>
+      <c r="B110" s="29"/>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="30"/>
+      <c r="B111" s="29"/>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="32"/>
+      <c r="B112" s="31"/>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="32"/>
+      <c r="B113" s="31"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="32"/>
+      <c r="B114" s="31"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="32"/>
+      <c r="B115" s="31"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="32"/>
+      <c r="B116" s="31"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="32"/>
+      <c r="B117" s="31"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="32"/>
+      <c r="B118" s="31"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="32"/>
+      <c r="B119" s="31"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="32"/>
+      <c r="B120" s="31"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="32"/>
+      <c r="B121" s="31"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="30"/>
+      <c r="B122" s="29"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="30"/>
+      <c r="B123" s="29"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="32"/>
+      <c r="B124" s="31"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="32"/>
+      <c r="B125" s="31"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="32"/>
+      <c r="B126" s="31"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="32"/>
+      <c r="B127" s="31"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="32"/>
+      <c r="B128" s="31"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B129" s="32"/>
+      <c r="B129" s="31"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="32"/>
+      <c r="B130" s="31"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B131" s="32"/>
+      <c r="B131" s="31"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B132" s="32"/>
+      <c r="B132" s="31"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B133" s="32"/>
+      <c r="B133" s="31"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B134" s="30"/>
+      <c r="B134" s="29"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B135" s="30"/>
+      <c r="B135" s="29"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B136" s="32"/>
+      <c r="B136" s="31"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B137" s="32"/>
+      <c r="B137" s="31"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="32"/>
+      <c r="B138" s="31"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B139" s="32"/>
+      <c r="B139" s="31"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B140" s="32"/>
+      <c r="B140" s="31"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B141" s="32"/>
+      <c r="B141" s="31"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B142" s="32"/>
+      <c r="B142" s="31"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B143" s="32"/>
+      <c r="B143" s="31"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B144" s="32"/>
+      <c r="B144" s="31"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B145" s="32"/>
+      <c r="B145" s="31"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B146" s="30"/>
+      <c r="B146" s="29"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B147" s="30"/>
+      <c r="B147" s="29"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="32"/>
+      <c r="B148" s="31"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="32"/>
+      <c r="B149" s="31"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="32"/>
+      <c r="B150" s="31"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="32"/>
+      <c r="B151" s="31"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="32"/>
+      <c r="B152" s="31"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="32"/>
+      <c r="B153" s="31"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="32"/>
+      <c r="B154" s="31"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B155" s="32"/>
+      <c r="B155" s="31"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B156" s="32"/>
+      <c r="B156" s="31"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="32"/>
+      <c r="B157" s="31"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B158" s="30"/>
+      <c r="B158" s="29"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="30"/>
+      <c r="B159" s="29"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B160" s="32"/>
+      <c r="B160" s="31"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B161" s="32"/>
+      <c r="B161" s="31"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B162" s="32"/>
+      <c r="B162" s="31"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B163" s="32"/>
+      <c r="B163" s="31"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B164" s="32"/>
+      <c r="B164" s="31"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B165" s="32"/>
+      <c r="B165" s="31"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
     </row>
     <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="32"/>
+      <c r="B166" s="31"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
     </row>
     <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B167" s="32"/>
+      <c r="B167" s="31"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
     </row>
     <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B168" s="32"/>
+      <c r="B168" s="31"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
     </row>
     <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B169" s="32"/>
+      <c r="B169" s="31"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
     </row>
     <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B170" s="30"/>
+      <c r="B170" s="29"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
     </row>
     <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B171" s="30"/>
+      <c r="B171" s="29"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
     </row>
     <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B172" s="32"/>
+      <c r="B172" s="31"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
     </row>
     <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B173" s="32"/>
+      <c r="B173" s="31"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
     </row>
     <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="32"/>
+      <c r="B174" s="31"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
     </row>
     <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B175" s="32"/>
+      <c r="B175" s="31"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
     </row>
     <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="32"/>
+      <c r="B176" s="31"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
     </row>
     <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B177" s="32"/>
+      <c r="B177" s="31"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
     </row>
     <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B178" s="32"/>
+      <c r="B178" s="31"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
     </row>
     <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B179" s="32"/>
+      <c r="B179" s="31"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
     </row>
     <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B180" s="32"/>
+      <c r="B180" s="31"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
     </row>
     <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B181" s="32"/>
+      <c r="B181" s="31"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
     </row>
@@ -2295,7 +2286,7 @@
   </sheetPr>
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
@@ -2486,7 +2477,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -2510,7 +2501,7 @@
       <c r="C1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>53</v>
       </c>
     </row>
@@ -2524,7 +2515,7 @@
       <c r="C2" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="36" t="n">
+      <c r="D2" s="35" t="n">
         <f aca="false">MAX(MAX('invoicing periods'!C2:C900),MAX(tasks!C2:C613))</f>
         <v>46391</v>
       </c>
@@ -2547,8 +2538,8 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K76" activeCellId="0" sqref="K76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2559,7 +2550,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2586,10 +2577,10 @@
       <c r="I1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2620,11 +2611,11 @@
       <c r="I2" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="J2" s="38" t="b">
+      <c r="J2" s="37" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="38" t="b">
+      <c r="K2" s="37" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -2647,7 +2638,7 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2658,7 +2649,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>65</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2685,10 +2676,10 @@
       <c r="I1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="35" t="s">
+      <c r="K1" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2719,11 +2710,11 @@
       <c r="I2" s="6" t="n">
         <v>0.3</v>
       </c>
-      <c r="J2" s="38" t="b">
+      <c r="J2" s="37" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="K2" s="38" t="b">
+      <c r="K2" s="37" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -2746,7 +2737,7 @@
   </sheetPr>
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2757,7 +2748,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2778,10 +2769,10 @@
       <c r="G1" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="34" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2806,11 +2797,11 @@
       <c r="G2" s="6" t="n">
         <v>0.6</v>
       </c>
-      <c r="H2" s="38" t="b">
+      <c r="H2" s="37" t="b">
         <f aca="false">AND(ISNUMBER(E2), E2&gt;misc!A2)</f>
         <v>1</v>
       </c>
-      <c r="I2" s="38" t="b">
+      <c r="I2" s="37" t="b">
         <f aca="false">AND(ISNUMBER(F2), E2&lt;=F2, F2&lt;=misc!D2)</f>
         <v>1</v>
       </c>
@@ -2836,7 +2827,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -2847,7 +2838,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>69</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2907,7 +2898,7 @@
   </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2918,7 +2909,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>74</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -2978,7 +2969,7 @@
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J30" activeCellId="0" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -2991,7 +2982,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>79</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -3069,8 +3060,8 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3318,35 +3309,33 @@
         <v>16</v>
       </c>
       <c r="B6" s="16" t="n">
-        <f aca="false">B3</f>
-        <v>45814</v>
+        <v>45698</v>
       </c>
       <c r="C6" s="16" t="n">
-        <f aca="false">C3</f>
-        <v>45844</v>
+        <v>45715</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E6" s="17" t="n">
         <f aca="false">C6 - B6 +1</f>
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F6" s="17" t="n">
         <f aca="false">NETWORKDAYS(B6, C6, 'public holidays'!A$2:A$500)</f>
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G6" s="18" t="n">
         <f aca="false">D6/F6</f>
-        <v>0.476190476190476</v>
+        <v>0.714285714285714</v>
       </c>
       <c r="H6" s="19" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G6, 0.25)</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="I6" s="19" t="n">
         <f aca="false">H6 + 0.25</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J6" s="2" t="b">
         <f aca="false">COUNTIF(links!$B$1:$B$493, A6) &gt; 0</f>
@@ -3367,33 +3356,33 @@
         <v>17</v>
       </c>
       <c r="B7" s="16" t="n">
-        <v>45698</v>
+        <v>45716</v>
       </c>
       <c r="C7" s="16" t="n">
-        <v>45715</v>
+        <v>45838</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>50</v>
       </c>
       <c r="E7" s="17" t="n">
         <f aca="false">C7 - B7 +1</f>
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="F7" s="17" t="n">
         <f aca="false">NETWORKDAYS(B7, C7, 'public holidays'!A$2:A$500)</f>
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="G7" s="18" t="n">
         <f aca="false">D7/F7</f>
-        <v>3.57142857142857</v>
+        <v>0.581395348837209</v>
       </c>
       <c r="H7" s="19" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G7, 0.25)</f>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="I7" s="19" t="n">
         <f aca="false">H7 + 0.25</f>
-        <v>3.75</v>
+        <v>0.75</v>
       </c>
       <c r="J7" s="2" t="b">
         <f aca="false">COUNTIF(links!$B$1:$B$493, A7) &gt; 0</f>
@@ -3414,25 +3403,25 @@
         <v>18</v>
       </c>
       <c r="B8" s="16" t="n">
-        <v>45716</v>
+        <v>45839</v>
       </c>
       <c r="C8" s="16" t="n">
-        <v>45838</v>
+        <v>45884</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>5</v>
       </c>
       <c r="E8" s="17" t="n">
         <f aca="false">C8 - B8 +1</f>
-        <v>123</v>
+        <v>46</v>
       </c>
       <c r="F8" s="17" t="n">
         <f aca="false">NETWORKDAYS(B8, C8, 'public holidays'!A$2:A$500)</f>
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="G8" s="18" t="n">
         <f aca="false">D8/F8</f>
-        <v>0.0581395348837209</v>
+        <v>0.147058823529412</v>
       </c>
       <c r="H8" s="19" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G8, 0.25)</f>
@@ -3461,33 +3450,33 @@
         <v>19</v>
       </c>
       <c r="B9" s="16" t="n">
-        <v>45839</v>
+        <v>45757</v>
       </c>
       <c r="C9" s="16" t="n">
-        <v>45884</v>
+        <v>45767</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>10</v>
       </c>
       <c r="E9" s="17" t="n">
         <f aca="false">C9 - B9 +1</f>
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="F9" s="17" t="n">
         <f aca="false">NETWORKDAYS(B9, C9, 'public holidays'!A$2:A$500)</f>
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G9" s="18" t="n">
         <f aca="false">D9/F9</f>
-        <v>0.294117647058824</v>
+        <v>1.42857142857143</v>
       </c>
       <c r="H9" s="19" t="n">
         <f aca="false">_xlfn.FLOOR.MATH(G9, 0.25)</f>
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="I9" s="19" t="n">
         <f aca="false">H9 + 0.25</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="J9" s="2" t="b">
         <f aca="false">COUNTIF(links!$B$1:$B$493, A9) &gt; 0</f>
@@ -4190,7 +4179,7 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F59" activeCellId="0" sqref="F59"/>
     </sheetView>
   </sheetViews>
@@ -4973,8 +4962,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O24" activeCellId="0" sqref="O24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5182,11 +5171,11 @@
       </c>
       <c r="E6" s="24" t="n">
         <f aca="false">VLOOKUP(B6, tasks!A$2:I$23, 8, 0)</f>
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F6" s="24" t="n">
         <f aca="false">VLOOKUP(B6, tasks!A$2:I$23, 9, 0)</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G6" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A6) &gt; 0</f>
@@ -5252,11 +5241,11 @@
       </c>
       <c r="E8" s="24" t="n">
         <f aca="false">VLOOKUP(B8, tasks!A$2:I$23, 8, 0)</f>
-        <v>3.5</v>
+        <v>0.5</v>
       </c>
       <c r="F8" s="24" t="n">
         <f aca="false">VLOOKUP(B8, tasks!A$2:I$23, 9, 0)</f>
-        <v>3.75</v>
+        <v>0.75</v>
       </c>
       <c r="G8" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A8) &gt; 0</f>
@@ -5286,11 +5275,11 @@
       </c>
       <c r="E9" s="24" t="n">
         <f aca="false">VLOOKUP(B9, tasks!A$2:I$23, 8, 0)</f>
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="F9" s="24" t="n">
         <f aca="false">VLOOKUP(B9, tasks!A$2:I$23, 9, 0)</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="G9" s="2" t="n">
         <f aca="false">COUNTIF(experts!$A$2:$A$954, A9) &gt; 0</f>
@@ -5836,7 +5825,6 @@
       <c r="J31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="28"/>
       <c r="C32" s="26"/>
       <c r="D32" s="26"/>
       <c r="E32" s="24"/>
@@ -6298,7 +6286,7 @@
   </sheetPr>
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -6323,10 +6311,10 @@
       <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -6693,7 +6681,7 @@
   </sheetPr>
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -6713,10 +6701,10 @@
       <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7152,7 +7140,7 @@
   </sheetPr>
   <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -7177,10 +7165,10 @@
       <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7547,7 +7535,7 @@
   </sheetPr>
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -7567,10 +7555,10 @@
       <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>11</v>
       </c>
     </row>
@@ -7744,8 +7732,8 @@
   </sheetPr>
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7771,13 +7759,13 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="31" t="n">
+      <c r="B2" s="30" t="n">
         <v>45637</v>
       </c>
-      <c r="C2" s="31" t="n">
+      <c r="C2" s="30" t="n">
         <v>45672</v>
       </c>
       <c r="D2" s="2" t="b">
@@ -7786,13 +7774,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="31" t="n">
+      <c r="B3" s="30" t="n">
         <v>45673</v>
       </c>
-      <c r="C3" s="31" t="n">
+      <c r="C3" s="30" t="n">
         <v>45701</v>
       </c>
       <c r="D3" s="2" t="n">
@@ -7801,13 +7789,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="33" t="n">
+      <c r="B4" s="32" t="n">
         <v>45702</v>
       </c>
-      <c r="C4" s="33" t="n">
+      <c r="C4" s="32" t="n">
         <v>45732</v>
       </c>
       <c r="D4" s="2" t="n">
@@ -7816,13 +7804,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="33" t="n">
+      <c r="B5" s="32" t="n">
         <v>45733</v>
       </c>
-      <c r="C5" s="33" t="n">
+      <c r="C5" s="32" t="n">
         <v>45761</v>
       </c>
       <c r="D5" s="2" t="n">
@@ -7831,13 +7819,13 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="33" t="n">
+      <c r="B6" s="32" t="n">
         <v>45762</v>
       </c>
-      <c r="C6" s="33" t="n">
+      <c r="C6" s="32" t="n">
         <v>45795</v>
       </c>
       <c r="D6" s="2" t="n">
@@ -7846,13 +7834,13 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="33" t="n">
+      <c r="B7" s="32" t="n">
         <v>45796</v>
       </c>
-      <c r="C7" s="33" t="n">
+      <c r="C7" s="32" t="n">
         <v>45826</v>
       </c>
       <c r="D7" s="2" t="n">
@@ -7861,13 +7849,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="16" t="n">
         <v>45827</v>
       </c>
-      <c r="C8" s="33" t="n">
+      <c r="C8" s="32" t="n">
         <v>45855</v>
       </c>
       <c r="D8" s="2" t="n">
@@ -7876,13 +7864,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="33" t="n">
+      <c r="B9" s="32" t="n">
         <v>45856</v>
       </c>
-      <c r="C9" s="33" t="n">
+      <c r="C9" s="32" t="n">
         <v>45886</v>
       </c>
       <c r="D9" s="2" t="n">
@@ -7891,7 +7879,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="31" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="16" t="n">
@@ -7906,7 +7894,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B11" s="16" t="n">
@@ -7921,7 +7909,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="31" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="16" t="n">
@@ -7936,7 +7924,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="31" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="16" t="n">

</xml_diff>